<commit_message>
upgrade with the saveashtml module to save Pulse code & prod
</commit_message>
<xml_diff>
--- a/output/dayforecastmob.xlsx
+++ b/output/dayforecastmob.xlsx
@@ -441,7 +441,7 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>10/03/2023</t>
+          <t>11/03/2023</t>
         </is>
       </c>
     </row>
@@ -450,7 +450,7 @@
         <v>8</v>
       </c>
       <c r="B2" t="n">
-        <v>138</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3">
@@ -458,7 +458,7 @@
         <v>9</v>
       </c>
       <c r="B3" t="n">
-        <v>209</v>
+        <v>136</v>
       </c>
     </row>
     <row r="4">
@@ -466,7 +466,7 @@
         <v>10</v>
       </c>
       <c r="B4" t="n">
-        <v>181</v>
+        <v>118</v>
       </c>
     </row>
     <row r="5">
@@ -474,7 +474,7 @@
         <v>11</v>
       </c>
       <c r="B5" t="n">
-        <v>175</v>
+        <v>110</v>
       </c>
     </row>
     <row r="6">
@@ -482,7 +482,7 @@
         <v>12</v>
       </c>
       <c r="B6" t="n">
-        <v>147</v>
+        <v>101</v>
       </c>
     </row>
     <row r="7">
@@ -490,7 +490,7 @@
         <v>13</v>
       </c>
       <c r="B7" t="n">
-        <v>133</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8">
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="B8" t="n">
-        <v>135</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9">
@@ -506,7 +506,7 @@
         <v>15</v>
       </c>
       <c r="B9" t="n">
-        <v>130</v>
+        <v>106</v>
       </c>
     </row>
     <row r="10">
@@ -514,7 +514,7 @@
         <v>16</v>
       </c>
       <c r="B10" t="n">
-        <v>140</v>
+        <v>88</v>
       </c>
     </row>
     <row r="11">
@@ -522,7 +522,7 @@
         <v>17</v>
       </c>
       <c r="B11" t="n">
-        <v>141</v>
+        <v>91</v>
       </c>
     </row>
     <row r="12">
@@ -530,7 +530,7 @@
         <v>18</v>
       </c>
       <c r="B12" t="n">
-        <v>151</v>
+        <v>77</v>
       </c>
     </row>
     <row r="13">
@@ -538,7 +538,7 @@
         <v>19</v>
       </c>
       <c r="B13" t="n">
-        <v>116</v>
+        <v>68</v>
       </c>
     </row>
     <row r="14">
@@ -546,7 +546,7 @@
         <v>20</v>
       </c>
       <c r="B14" t="n">
-        <v>76</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15">
@@ -554,7 +554,7 @@
         <v>21</v>
       </c>
       <c r="B15" t="n">
-        <v>49</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16">
@@ -562,7 +562,7 @@
         <v>22</v>
       </c>
       <c r="B16" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17">
@@ -570,7 +570,7 @@
         <v>23</v>
       </c>
       <c r="B17" t="n">
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
idea to refresh charts with matplotlib.animation
</commit_message>
<xml_diff>
--- a/output/dayforecastmob.xlsx
+++ b/output/dayforecastmob.xlsx
@@ -441,7 +441,7 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>11/03/2023</t>
+          <t>14/03/2023</t>
         </is>
       </c>
     </row>
@@ -450,7 +450,7 @@
         <v>8</v>
       </c>
       <c r="B2" t="n">
-        <v>66</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3">
@@ -458,7 +458,7 @@
         <v>9</v>
       </c>
       <c r="B3" t="n">
-        <v>136</v>
+        <v>165</v>
       </c>
     </row>
     <row r="4">
@@ -466,7 +466,7 @@
         <v>10</v>
       </c>
       <c r="B4" t="n">
-        <v>118</v>
+        <v>218</v>
       </c>
     </row>
     <row r="5">
@@ -474,7 +474,7 @@
         <v>11</v>
       </c>
       <c r="B5" t="n">
-        <v>110</v>
+        <v>213</v>
       </c>
     </row>
     <row r="6">
@@ -482,7 +482,7 @@
         <v>12</v>
       </c>
       <c r="B6" t="n">
-        <v>101</v>
+        <v>179</v>
       </c>
     </row>
     <row r="7">
@@ -490,7 +490,7 @@
         <v>13</v>
       </c>
       <c r="B7" t="n">
-        <v>87</v>
+        <v>148</v>
       </c>
     </row>
     <row r="8">
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="B8" t="n">
-        <v>84</v>
+        <v>166</v>
       </c>
     </row>
     <row r="9">
@@ -506,7 +506,7 @@
         <v>15</v>
       </c>
       <c r="B9" t="n">
-        <v>106</v>
+        <v>145</v>
       </c>
     </row>
     <row r="10">
@@ -514,7 +514,7 @@
         <v>16</v>
       </c>
       <c r="B10" t="n">
-        <v>88</v>
+        <v>153</v>
       </c>
     </row>
     <row r="11">
@@ -522,7 +522,7 @@
         <v>17</v>
       </c>
       <c r="B11" t="n">
-        <v>91</v>
+        <v>162</v>
       </c>
     </row>
     <row r="12">
@@ -530,7 +530,7 @@
         <v>18</v>
       </c>
       <c r="B12" t="n">
-        <v>77</v>
+        <v>155</v>
       </c>
     </row>
     <row r="13">
@@ -538,7 +538,7 @@
         <v>19</v>
       </c>
       <c r="B13" t="n">
-        <v>68</v>
+        <v>129</v>
       </c>
     </row>
     <row r="14">
@@ -546,7 +546,7 @@
         <v>20</v>
       </c>
       <c r="B14" t="n">
-        <v>53</v>
+        <v>78</v>
       </c>
     </row>
     <row r="15">
@@ -554,7 +554,7 @@
         <v>21</v>
       </c>
       <c r="B15" t="n">
-        <v>22</v>
+        <v>48</v>
       </c>
     </row>
     <row r="16">
@@ -562,7 +562,7 @@
         <v>22</v>
       </c>
       <c r="B16" t="n">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17">

</xml_diff>

<commit_message>
initiate the real timeframe recording of calls
</commit_message>
<xml_diff>
--- a/output/dayforecastmob.xlsx
+++ b/output/dayforecastmob.xlsx
@@ -441,7 +441,7 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>14/03/2023</t>
+          <t>18/03/2023</t>
         </is>
       </c>
     </row>
@@ -450,7 +450,7 @@
         <v>8</v>
       </c>
       <c r="B2" t="n">
-        <v>82</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3">
@@ -458,7 +458,7 @@
         <v>9</v>
       </c>
       <c r="B3" t="n">
-        <v>165</v>
+        <v>153</v>
       </c>
     </row>
     <row r="4">
@@ -466,7 +466,7 @@
         <v>10</v>
       </c>
       <c r="B4" t="n">
-        <v>218</v>
+        <v>128</v>
       </c>
     </row>
     <row r="5">
@@ -474,7 +474,7 @@
         <v>11</v>
       </c>
       <c r="B5" t="n">
-        <v>213</v>
+        <v>117</v>
       </c>
     </row>
     <row r="6">
@@ -482,7 +482,7 @@
         <v>12</v>
       </c>
       <c r="B6" t="n">
-        <v>179</v>
+        <v>109</v>
       </c>
     </row>
     <row r="7">
@@ -490,7 +490,7 @@
         <v>13</v>
       </c>
       <c r="B7" t="n">
-        <v>148</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8">
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="B8" t="n">
-        <v>166</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9">
@@ -506,7 +506,7 @@
         <v>15</v>
       </c>
       <c r="B9" t="n">
-        <v>145</v>
+        <v>118</v>
       </c>
     </row>
     <row r="10">
@@ -514,7 +514,7 @@
         <v>16</v>
       </c>
       <c r="B10" t="n">
-        <v>153</v>
+        <v>97</v>
       </c>
     </row>
     <row r="11">
@@ -522,7 +522,7 @@
         <v>17</v>
       </c>
       <c r="B11" t="n">
-        <v>162</v>
+        <v>99</v>
       </c>
     </row>
     <row r="12">
@@ -530,7 +530,7 @@
         <v>18</v>
       </c>
       <c r="B12" t="n">
-        <v>155</v>
+        <v>85</v>
       </c>
     </row>
     <row r="13">
@@ -538,7 +538,7 @@
         <v>19</v>
       </c>
       <c r="B13" t="n">
-        <v>129</v>
+        <v>76</v>
       </c>
     </row>
     <row r="14">
@@ -546,7 +546,7 @@
         <v>20</v>
       </c>
       <c r="B14" t="n">
-        <v>78</v>
+        <v>61</v>
       </c>
     </row>
     <row r="15">
@@ -554,7 +554,7 @@
         <v>21</v>
       </c>
       <c r="B15" t="n">
-        <v>48</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16">
@@ -562,7 +562,7 @@
         <v>22</v>
       </c>
       <c r="B16" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17">
@@ -570,7 +570,7 @@
         <v>23</v>
       </c>
       <c r="B17" t="n">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update dayrealmob correct cell in time
</commit_message>
<xml_diff>
--- a/output/dayforecastmob.xlsx
+++ b/output/dayforecastmob.xlsx
@@ -441,7 +441,7 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>18/03/2023</t>
+          <t>21/03/2023</t>
         </is>
       </c>
     </row>
@@ -450,7 +450,7 @@
         <v>8</v>
       </c>
       <c r="B2" t="n">
-        <v>73</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3">
@@ -458,7 +458,7 @@
         <v>9</v>
       </c>
       <c r="B3" t="n">
-        <v>153</v>
+        <v>180</v>
       </c>
     </row>
     <row r="4">
@@ -466,7 +466,7 @@
         <v>10</v>
       </c>
       <c r="B4" t="n">
-        <v>128</v>
+        <v>235</v>
       </c>
     </row>
     <row r="5">
@@ -474,7 +474,7 @@
         <v>11</v>
       </c>
       <c r="B5" t="n">
-        <v>117</v>
+        <v>229</v>
       </c>
     </row>
     <row r="6">
@@ -482,7 +482,7 @@
         <v>12</v>
       </c>
       <c r="B6" t="n">
-        <v>109</v>
+        <v>193</v>
       </c>
     </row>
     <row r="7">
@@ -490,7 +490,7 @@
         <v>13</v>
       </c>
       <c r="B7" t="n">
-        <v>93</v>
+        <v>159</v>
       </c>
     </row>
     <row r="8">
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="B8" t="n">
-        <v>91</v>
+        <v>180</v>
       </c>
     </row>
     <row r="9">
@@ -506,7 +506,7 @@
         <v>15</v>
       </c>
       <c r="B9" t="n">
-        <v>118</v>
+        <v>156</v>
       </c>
     </row>
     <row r="10">
@@ -514,7 +514,7 @@
         <v>16</v>
       </c>
       <c r="B10" t="n">
-        <v>97</v>
+        <v>165</v>
       </c>
     </row>
     <row r="11">
@@ -522,7 +522,7 @@
         <v>17</v>
       </c>
       <c r="B11" t="n">
-        <v>99</v>
+        <v>175</v>
       </c>
     </row>
     <row r="12">
@@ -530,7 +530,7 @@
         <v>18</v>
       </c>
       <c r="B12" t="n">
-        <v>85</v>
+        <v>167</v>
       </c>
     </row>
     <row r="13">
@@ -538,7 +538,7 @@
         <v>19</v>
       </c>
       <c r="B13" t="n">
-        <v>76</v>
+        <v>140</v>
       </c>
     </row>
     <row r="14">
@@ -546,7 +546,7 @@
         <v>20</v>
       </c>
       <c r="B14" t="n">
-        <v>61</v>
+        <v>83</v>
       </c>
     </row>
     <row r="15">
@@ -554,7 +554,7 @@
         <v>21</v>
       </c>
       <c r="B15" t="n">
-        <v>24</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16">
@@ -562,7 +562,7 @@
         <v>22</v>
       </c>
       <c r="B16" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17">
@@ -570,7 +570,7 @@
         <v>23</v>
       </c>
       <c r="B17" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
draft of refreshig realtime offerte --> ok
</commit_message>
<xml_diff>
--- a/output/dayforecastmob.xlsx
+++ b/output/dayforecastmob.xlsx
@@ -441,7 +441,7 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>21/03/2023</t>
+          <t>24/03/2023</t>
         </is>
       </c>
     </row>
@@ -450,7 +450,7 @@
         <v>8</v>
       </c>
       <c r="B2" t="n">
-        <v>89</v>
+        <v>148</v>
       </c>
     </row>
     <row r="3">
@@ -458,7 +458,7 @@
         <v>9</v>
       </c>
       <c r="B3" t="n">
-        <v>180</v>
+        <v>221</v>
       </c>
     </row>
     <row r="4">
@@ -466,7 +466,7 @@
         <v>10</v>
       </c>
       <c r="B4" t="n">
-        <v>235</v>
+        <v>189</v>
       </c>
     </row>
     <row r="5">
@@ -474,7 +474,7 @@
         <v>11</v>
       </c>
       <c r="B5" t="n">
-        <v>229</v>
+        <v>180</v>
       </c>
     </row>
     <row r="6">
@@ -482,7 +482,7 @@
         <v>12</v>
       </c>
       <c r="B6" t="n">
-        <v>193</v>
+        <v>153</v>
       </c>
     </row>
     <row r="7">
@@ -490,7 +490,7 @@
         <v>13</v>
       </c>
       <c r="B7" t="n">
-        <v>159</v>
+        <v>137</v>
       </c>
     </row>
     <row r="8">
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="B8" t="n">
-        <v>180</v>
+        <v>140</v>
       </c>
     </row>
     <row r="9">
@@ -506,7 +506,7 @@
         <v>15</v>
       </c>
       <c r="B9" t="n">
-        <v>156</v>
+        <v>134</v>
       </c>
     </row>
     <row r="10">
@@ -514,7 +514,7 @@
         <v>16</v>
       </c>
       <c r="B10" t="n">
-        <v>165</v>
+        <v>145</v>
       </c>
     </row>
     <row r="11">
@@ -522,7 +522,7 @@
         <v>17</v>
       </c>
       <c r="B11" t="n">
-        <v>175</v>
+        <v>146</v>
       </c>
     </row>
     <row r="12">
@@ -530,7 +530,7 @@
         <v>18</v>
       </c>
       <c r="B12" t="n">
-        <v>167</v>
+        <v>157</v>
       </c>
     </row>
     <row r="13">
@@ -538,7 +538,7 @@
         <v>19</v>
       </c>
       <c r="B13" t="n">
-        <v>140</v>
+        <v>122</v>
       </c>
     </row>
     <row r="14">
@@ -546,7 +546,7 @@
         <v>20</v>
       </c>
       <c r="B14" t="n">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="15">
@@ -554,7 +554,7 @@
         <v>21</v>
       </c>
       <c r="B15" t="n">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="16">
@@ -562,7 +562,7 @@
         <v>22</v>
       </c>
       <c r="B16" t="n">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17">
@@ -570,7 +570,7 @@
         <v>23</v>
       </c>
       <c r="B17" t="n">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
correctly updating chart every frame and every hour
</commit_message>
<xml_diff>
--- a/output/dayforecastmob.xlsx
+++ b/output/dayforecastmob.xlsx
@@ -441,7 +441,7 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>24/03/2023</t>
+          <t>25/03/2023</t>
         </is>
       </c>
     </row>
@@ -450,7 +450,7 @@
         <v>8</v>
       </c>
       <c r="B2" t="n">
-        <v>148</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3">
@@ -458,7 +458,7 @@
         <v>9</v>
       </c>
       <c r="B3" t="n">
-        <v>221</v>
+        <v>167</v>
       </c>
     </row>
     <row r="4">
@@ -466,7 +466,7 @@
         <v>10</v>
       </c>
       <c r="B4" t="n">
-        <v>189</v>
+        <v>138</v>
       </c>
     </row>
     <row r="5">
@@ -474,7 +474,7 @@
         <v>11</v>
       </c>
       <c r="B5" t="n">
-        <v>180</v>
+        <v>125</v>
       </c>
     </row>
     <row r="6">
@@ -482,7 +482,7 @@
         <v>12</v>
       </c>
       <c r="B6" t="n">
-        <v>153</v>
+        <v>116</v>
       </c>
     </row>
     <row r="7">
@@ -490,7 +490,7 @@
         <v>13</v>
       </c>
       <c r="B7" t="n">
-        <v>137</v>
+        <v>99</v>
       </c>
     </row>
     <row r="8">
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="B8" t="n">
-        <v>140</v>
+        <v>98</v>
       </c>
     </row>
     <row r="9">
@@ -506,7 +506,7 @@
         <v>15</v>
       </c>
       <c r="B9" t="n">
-        <v>134</v>
+        <v>127</v>
       </c>
     </row>
     <row r="10">
@@ -514,7 +514,7 @@
         <v>16</v>
       </c>
       <c r="B10" t="n">
-        <v>145</v>
+        <v>105</v>
       </c>
     </row>
     <row r="11">
@@ -522,7 +522,7 @@
         <v>17</v>
       </c>
       <c r="B11" t="n">
-        <v>146</v>
+        <v>105</v>
       </c>
     </row>
     <row r="12">
@@ -530,7 +530,7 @@
         <v>18</v>
       </c>
       <c r="B12" t="n">
-        <v>157</v>
+        <v>91</v>
       </c>
     </row>
     <row r="13">
@@ -538,7 +538,7 @@
         <v>19</v>
       </c>
       <c r="B13" t="n">
-        <v>122</v>
+        <v>82</v>
       </c>
     </row>
     <row r="14">
@@ -546,7 +546,7 @@
         <v>20</v>
       </c>
       <c r="B14" t="n">
-        <v>80</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15">
@@ -554,7 +554,7 @@
         <v>21</v>
       </c>
       <c r="B15" t="n">
-        <v>51</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16">
@@ -562,7 +562,7 @@
         <v>22</v>
       </c>
       <c r="B16" t="n">
-        <v>19</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17">
@@ -570,7 +570,7 @@
         <v>23</v>
       </c>
       <c r="B17" t="n">
-        <v>12</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
alligned hour as index for chart ..> startin from 9 + records of pasthour update only at 00. ELiminated initialization
</commit_message>
<xml_diff>
--- a/output/dayforecastmob.xlsx
+++ b/output/dayforecastmob.xlsx
@@ -441,136 +441,136 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>25/03/2023</t>
+          <t>07/04/2023</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B2" t="n">
-        <v>78</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" t="n">
-        <v>167</v>
+        <v>200</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B4" t="n">
-        <v>138</v>
+        <v>236</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B5" t="n">
-        <v>125</v>
+        <v>214</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B6" t="n">
-        <v>116</v>
+        <v>168</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B7" t="n">
-        <v>99</v>
+        <v>133</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B8" t="n">
-        <v>98</v>
+        <v>129</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B9" t="n">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B10" t="n">
-        <v>105</v>
+        <v>132</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B11" t="n">
-        <v>105</v>
+        <v>135</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B12" t="n">
-        <v>91</v>
+        <v>132</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B13" t="n">
-        <v>82</v>
+        <v>104</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B14" t="n">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B15" t="n">
-        <v>27</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="B16" t="n">
         <v>22</v>
-      </c>
-      <c r="B16" t="n">
-        <v>27</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B17" t="n">
-        <v>22</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>